<commit_message>
Added readRoutes() and busRoutes()
</commit_message>
<xml_diff>
--- a/LSuperior/Schedule/Schedule_Info_LS.xlsx
+++ b/LSuperior/Schedule/Schedule_Info_LS.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaWork\Research\Creel_WiDNR\LSuperior\Schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaaWork\Research\WiDNR_Creel\LSuperior\Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Routes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +42,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="I17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Check these</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Check these</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -68,19 +94,55 @@
         </r>
       </text>
     </comment>
+    <comment ref="I19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Check these</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Check these</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Check these</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="38">
   <si>
     <t>route</t>
   </si>
   <si>
-    <t>period</t>
-  </si>
-  <si>
     <t>site_no</t>
   </si>
   <si>
@@ -174,26 +236,29 @@
     <t>West End</t>
   </si>
   <si>
-    <t>travel_order</t>
-  </si>
-  <si>
-    <t>travel_time</t>
-  </si>
-  <si>
-    <t>perc_effort</t>
-  </si>
-  <si>
     <t>Red Cliff</t>
   </si>
   <si>
     <t>Little Sand Bay</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>peffort</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>visit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,13 +272,63 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -228,8 +343,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,65 +636,69 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -585,22 +712,22 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
+      <c r="D3" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E3">
         <v>270</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -614,22 +741,22 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E4">
         <v>258</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -643,22 +770,22 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E5">
         <v>234</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -672,22 +799,22 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="E6">
         <v>204</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -701,22 +828,22 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -730,22 +857,22 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E8">
         <v>270</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -759,22 +886,22 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E9">
         <v>258</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -788,22 +915,22 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E10">
         <v>234</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -817,22 +944,22 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E11">
         <v>204</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11">
         <v>5</v>
@@ -846,22 +973,22 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E12">
         <v>363</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -875,22 +1002,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E13">
         <v>370</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -904,22 +1031,22 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E14">
         <v>501</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G14">
         <v>3</v>
@@ -933,22 +1060,22 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E15">
         <v>363</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -962,22 +1089,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E16">
         <v>370</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -991,22 +1118,22 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="E17">
         <v>520</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1015,56 +1142,56 @@
         <v>15</v>
       </c>
       <c r="I17">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="E18">
         <v>540</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="H18">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I18">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="E19">
         <v>545</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -1073,119 +1200,186 @@
         <v>12</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="E20">
         <v>555</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20">
         <v>4</v>
       </c>
+      <c r="H20">
+        <v>35</v>
+      </c>
       <c r="I20">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>999</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>100</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22">
+        <v>998</v>
+      </c>
+      <c r="F22" t="s">
         <v>28</v>
-      </c>
-      <c r="F22" t="s">
-        <v>29</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>997</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>996</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24">
         <v>3</v>
       </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>995</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25">
         <v>4</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More work on scheduler
</commit_message>
<xml_diff>
--- a/LSuperior/Schedule/Schedule_Info_LS.xlsx
+++ b/LSuperior/Schedule/Schedule_Info_LS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Routes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="86">
   <si>
     <t>route</t>
   </si>
@@ -246,6 +246,45 @@
   </si>
   <si>
     <t>Shift start time (military)</t>
+  </si>
+  <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>13:30</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>6:30</t>
+  </si>
+  <si>
+    <t>5:30</t>
+  </si>
+  <si>
+    <t>6:00</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>10:30</t>
+  </si>
+  <si>
+    <t>17:30</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>20:30</t>
+  </si>
+  <si>
+    <t>21:30</t>
   </si>
 </sst>
 </file>
@@ -363,7 +402,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -372,6 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,7 +694,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="E1" sqref="E1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>25</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1544,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1555,7 +1594,7 @@
     <col min="3" max="3" width="34.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.44140625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1597,11 +1636,11 @@
       <c r="E2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G2" s="13">
-        <v>0.5625</v>
+      <c r="F2" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1620,11 +1659,11 @@
       <c r="E3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G3" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1637,17 +1676,17 @@
       <c r="C4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G4" s="13">
-        <v>0.58333333333333337</v>
+      <c r="F4" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1660,17 +1699,17 @@
       <c r="C5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G5" s="13">
-        <v>0.875</v>
+      <c r="F5" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1683,17 +1722,17 @@
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G6" s="13">
-        <v>0.5625</v>
+      <c r="F6" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1706,17 +1745,17 @@
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F7" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1729,17 +1768,17 @@
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G8" s="13">
-        <v>0.58333333333333337</v>
+      <c r="F8" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1752,17 +1791,17 @@
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0.875</v>
+      <c r="F9" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1775,17 +1814,17 @@
       <c r="C10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0.5625</v>
+      <c r="F10" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1798,17 +1837,17 @@
       <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F11" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1821,17 +1860,17 @@
       <c r="C12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0.58333333333333337</v>
+      <c r="F12" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1844,17 +1883,17 @@
       <c r="C13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0.875</v>
+      <c r="F13" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1867,17 +1906,17 @@
       <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0.5625</v>
+      <c r="F14" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1890,17 +1929,17 @@
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G15" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F15" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1913,17 +1952,17 @@
       <c r="C16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G16" s="13">
-        <v>0.58333333333333337</v>
+      <c r="F16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1936,17 +1975,17 @@
       <c r="C17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G17" s="13">
-        <v>0.875</v>
+      <c r="F17" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1965,11 +2004,11 @@
       <c r="E18" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G18" s="13">
-        <v>0.5625</v>
+      <c r="F18" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1988,11 +2027,11 @@
       <c r="E19" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G19" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F19" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2011,11 +2050,11 @@
       <c r="E20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="13">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="G20" s="13">
-        <v>0.5625</v>
+      <c r="F20" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -2034,11 +2073,11 @@
       <c r="E21" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G21" s="13">
-        <v>0.85416666666666663</v>
+      <c r="F21" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2057,11 +2096,11 @@
       <c r="E22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="13">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="G22" s="13">
-        <v>0.5625</v>
+      <c r="F22" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -2080,11 +2119,11 @@
       <c r="E23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G23" s="13">
-        <v>0.89583333333333337</v>
+      <c r="F23" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2103,11 +2142,11 @@
       <c r="E24" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="G24" s="13">
-        <v>0.5625</v>
+      <c r="F24" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2126,11 +2165,11 @@
       <c r="E25" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G25" s="13">
-        <v>0.875</v>
+      <c r="F25" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2149,11 +2188,11 @@
       <c r="E26" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="13">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="G26" s="13">
-        <v>0.5625</v>
+      <c r="F26" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2172,11 +2211,11 @@
       <c r="E27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G27" s="13">
-        <v>0.85416666666666663</v>
+      <c r="F27" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2189,17 +2228,17 @@
       <c r="C28" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="20" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G28" s="13">
-        <v>0.5625</v>
+      <c r="F28" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -2212,17 +2251,17 @@
       <c r="C29" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="20" t="s">
         <v>35</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="13">
-        <v>0.5625</v>
-      </c>
-      <c r="G29" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F29" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -2235,17 +2274,17 @@
       <c r="C30" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="20" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="13">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G30" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F30" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2264,11 +2303,11 @@
       <c r="E31" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="13">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G31" s="13">
-        <v>0.875</v>
+      <c r="F31" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -2287,11 +2326,11 @@
       <c r="E32" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G32" s="13">
-        <v>0.58333333333333337</v>
+      <c r="F32" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2310,11 +2349,11 @@
       <c r="E33" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G33" s="13">
-        <v>0.875</v>
+      <c r="F33" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2333,11 +2372,11 @@
       <c r="E34" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F34" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G34" s="13">
-        <v>0.58333333333333337</v>
+      <c r="F34" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2356,11 +2395,11 @@
       <c r="E35" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G35" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F35" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2379,11 +2418,11 @@
       <c r="E36" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G36" s="13">
-        <v>0.875</v>
+      <c r="F36" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2402,11 +2441,11 @@
       <c r="E37" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F37" s="13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="G37" s="13">
-        <v>0.4375</v>
+      <c r="F37" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2425,11 +2464,11 @@
       <c r="E38" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="13">
-        <v>0.4375</v>
-      </c>
-      <c r="G38" s="13">
-        <v>0.58333333333333337</v>
+      <c r="F38" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2448,11 +2487,11 @@
       <c r="E39" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F39" s="13">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G39" s="13">
-        <v>0.72916666666666663</v>
+      <c r="F39" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2471,11 +2510,11 @@
       <c r="E40" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F40" s="13">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="G40" s="13">
-        <v>0.83333333333333337</v>
+      <c r="F40" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2494,11 +2533,11 @@
       <c r="E41" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F41" s="13">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="G41" s="13">
-        <v>0.875</v>
+      <c r="F41" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2511,7 +2550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update before major changes
</commit_message>
<xml_diff>
--- a/LSuperior/Schedule/Schedule_Info_LS.xlsx
+++ b/LSuperior/Schedule/Schedule_Info_LS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Clerks" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Routes_Meta" sheetId="3" r:id="rId4"/>
     <sheet name="Shifts" sheetId="2" r:id="rId5"/>
     <sheet name="Shifts_Meta" sheetId="4" r:id="rId6"/>
+    <sheet name="Shifts_OLD" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="95">
   <si>
     <t>route</t>
   </si>
@@ -337,7 +338,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +393,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -405,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -413,7 +426,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -426,6 +438,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,17 +723,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -739,87 +754,87 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>100</v>
       </c>
     </row>
@@ -843,7 +858,7 @@
     <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -855,7 +870,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -866,7 +881,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -876,31 +891,31 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>92</v>
       </c>
@@ -908,11 +923,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
         <v>43472</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>91</v>
       </c>
     </row>
@@ -923,10 +938,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,53 +998,53 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>301</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>2</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>297</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>3</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
-      <c r="G4" s="8">
-        <v>2</v>
+      <c r="G4" s="7">
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1049,7 +1064,7 @@
         <v>4</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -1072,10 +1087,10 @@
         <v>5</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1095,7 +1110,7 @@
         <v>6</v>
       </c>
       <c r="F7">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -1121,7 +1136,7 @@
         <v>32</v>
       </c>
       <c r="G8">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1144,7 +1159,7 @@
         <v>10</v>
       </c>
       <c r="G9">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1167,7 +1182,7 @@
         <v>15</v>
       </c>
       <c r="G10">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1190,7 +1205,7 @@
         <v>25</v>
       </c>
       <c r="G11">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1198,22 +1213,22 @@
         <v>15</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12">
-        <v>520</v>
+        <v>555</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G12">
-        <v>49.69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1221,13 +1236,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -1236,7 +1251,7 @@
         <v>8</v>
       </c>
       <c r="G13">
-        <v>1.56</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1244,19 +1259,19 @@
         <v>15</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14">
         <v>3</v>
       </c>
       <c r="F14">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <v>10</v>
@@ -1267,13 +1282,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15">
-        <v>555</v>
+        <v>520</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1282,167 +1297,75 @@
         <v>35</v>
       </c>
       <c r="G15">
-        <v>38.75</v>
+        <v>39.75</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>73</v>
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="C16">
-        <v>520</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>49.71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>73</v>
+      <c r="A17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C17">
-        <v>540</v>
+        <v>903</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>1.43</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>73</v>
+      <c r="A18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C18">
-        <v>545</v>
+        <v>905</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>9.7100000000000009</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19">
-        <v>555</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="F19">
-        <v>35</v>
-      </c>
-      <c r="G19">
-        <v>39.14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21">
-        <v>903</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>10</v>
-      </c>
-      <c r="G21">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22">
-        <v>905</v>
-      </c>
-      <c r="D22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>10</v>
-      </c>
-      <c r="G22">
         <v>20</v>
       </c>
     </row>
@@ -1479,7 +1402,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -1487,7 +1410,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B3" t="s">
@@ -1495,7 +1418,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -1503,7 +1426,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -1511,7 +1434,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
@@ -1519,7 +1442,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
@@ -1527,7 +1450,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B8" t="s">
@@ -1543,7 +1466,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+      <c r="A12" s="18">
         <v>43472</v>
       </c>
       <c r="B12" t="s">
@@ -1551,7 +1474,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>43472</v>
       </c>
       <c r="B13" t="s">
@@ -1566,18 +1489,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="17"/>
+    <col min="1" max="1" width="34.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1598,206 +1521,206 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1805,16 +1728,16 @@
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1822,16 +1745,16 @@
       <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1839,16 +1762,16 @@
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1856,16 +1779,16 @@
       <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1873,16 +1796,16 @@
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1890,16 +1813,16 @@
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1907,16 +1830,16 @@
       <c r="A20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1924,16 +1847,16 @@
       <c r="A21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1941,16 +1864,16 @@
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1958,258 +1881,91 @@
       <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="16" t="s">
+      <c r="A24" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="16" t="s">
+      <c r="A25" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="17" t="s">
+      <c r="C25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>65</v>
+      <c r="A26" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="17" t="s">
+      <c r="A27" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:E23">
+    <sortCondition ref="A2:A23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2241,23 +1997,23 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B4" t="s">
@@ -2265,7 +2021,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B5" t="s">
@@ -2273,14 +2029,14 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>92</v>
       </c>
@@ -2288,12 +2044,288 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+    <row r="11" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
         <v>43472</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>